<commit_message>
Change Timeout / Foul
>Change Foul data display to display "P" on 8 & 9 fouls in main display only.

When Team Fouls in controller reaches 8 and 9, display blank (F data) in main display iso that the "P" (for penalty) will the only one be seen in main display.

>Change Team Remaining Timeout zero to blank in main display only.

When Team Remaining Timeouts become zero, blank (F data)should be shown instead so that no dots will be shown in main display i.e. 4dots --> 3dots --> 2dots --> 1dots --> Blank.
</commit_message>
<xml_diff>
--- a/trianScoreBoard_Issue_List.xlsx
+++ b/trianScoreBoard_Issue_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jezreel Tan\Desktop\Scoreboard_Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1320C1E8-4322-4139-ABAF-AA64709B0708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4573F21-68B7-46CD-8419-4CB1B2B6D6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>No.</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>Instead of only 0 to 4 period, add "E" after 4 for extended period situation both in controller &amp; main displays.</t>
-  </si>
-  <si>
-    <t>FINISHED</t>
   </si>
 </sst>
 </file>
@@ -215,7 +212,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,25 +227,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +265,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -291,32 +276,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -626,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,14 +737,14 @@
       <c r="CV1" s="3"/>
     </row>
     <row r="2" spans="1:100" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -862,250 +844,228 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:100" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:100" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:100" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:100" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E7" s="4"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:100" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:100" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:100" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:100" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:100" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:100" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:100" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:100" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:100" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1113,47 +1073,46 @@
       <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>

</xml_diff>

<commit_message>
Option for switcheable Wifi
A0 analog input. Connect to 3.3v for HIGH
Update README.md
</commit_message>
<xml_diff>
--- a/trianScoreBoard_Issue_List.xlsx
+++ b/trianScoreBoard_Issue_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jezreel Tan\Desktop\Scoreboard_Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4573F21-68B7-46CD-8419-4CB1B2B6D6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B70BF5-2A93-48FC-B2C6-78FAE46C4752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
   <dimension ref="A1:CV96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,13 +1088,13 @@
       <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="4"/>

</xml_diff>